<commit_message>
Feat zip file max size
</commit_message>
<xml_diff>
--- a/excel-files/keywords/keywords-list.xlsx
+++ b/excel-files/keywords/keywords-list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,43 +441,919 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Keywords</t>
+          <t>Marca</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Categoria</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tocador Contemporáneo Vico Blanco 210 cm TU MESITA</t>
+          <t xml:space="preserve">Gabinete de Baño Alden Muebles Gaudi </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lo siento, pero no puedo generar keywords comerciales</t>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>gabinete, bao, alden, muebles, gaudi, organización de baño</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tocador Contemporáneo Colucci Blanco 230 cm TU MESITA</t>
+          <t>Gabinete de Baño Alden Blanco Muebles Gaudi</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Inmobiliario, Tocador contemporáneo, Tocador TU MESITA, Tocadores y Percheros, Decoración del hogar, muebles, tocadores blancos, decoración de baño moderna</t>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>gabinete, bao, alden, blanco, muebles, gaudi, organización de baño</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tocador Contemporáneo Federal Blanco Negro 150cm TU MESITA</t>
+          <t>Gabinete de Baño Alden Negro Muebles Gaudi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lo siento, pero no puedo generar una lista completa de keywords comerciales para el producto</t>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>gabinete, bao, alden, negro, muebles, gaudi, organización de baño</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Gabinete de Baño Beckett Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>gabinete, bao, beckett, muebles, gaudi, organización de baño</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Gabinete de Baño Beckett Grafito Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>gabinete, bao, beckett, grafito, muebles, gaudi, organización de baño</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Gabinete de Baño Brooks Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>gabinete, bao, brooks, muebles, gaudi, organización de baño</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Gabinete de Baño Byron Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>gabinete, bao, byron, muebles, gaudi, organización de baño</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Gabinete de Baño Calvin Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>gabinete, bao, calvin, muebles, gaudi, organización de baño</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Gabinete de Baño Cormac Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>gabinete, bao, cormac, muebles, gaudi, organización de baño</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Gabinete de Baño Dashiell Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Organización de Baño</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>gabinete, bao, dashiell, muebles, gaudi, organización de baño</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Velador Dexter Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>velador, dexter, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Velador Dexter Blanco Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>velador, dexter, blanco, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Velador Dexter Duna Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>velador, dexter, duna, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Velador Dexter Grafito Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>velador, dexter, grafito, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Velador Huck Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>velador, huck, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Velador Huck Habano Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>velador, huck, habano, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Velador Jack Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>velador, jack, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Velador Jack Oceano Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>velador, jack, oceano, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Velador Jack Negro Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>velador, jack, negro, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Velador Jett Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>velador, jett, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Velador Jett Blanco Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>velador, jett, blanco, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Velador Jett Duna Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>velador, jett, duna, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Velador Lincoln Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>velador, lincoln, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Velador Lincoln Blanco Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>velador, lincoln, blanco, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Velador Mavel Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>velador, mavel, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Velador Mavel Amazónico Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Veladores</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>velador, mavel, amazónico, muebles, gaudi, veladores</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Tocador Monty Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>tocador, monty, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Tocador Monty Negro Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>tocador, monty, negro, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Tocador Orson Premium Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>tocador, orson, premium, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Tocador Otis Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>tocador, otis, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Tocador Infantil Ryder Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>tocador, infantil, ryder, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Tocador Infantil Ryder Rosa Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>tocador, infantil, ryder, rosa, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Tocador Sullivan Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>tocador, sullivan, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Tocador Waldo Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>tocador, waldo, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Tocador Portatil Watson Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>tocador, portatil, watson, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Tocador Zane Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>tocador, zane, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Tocador Premium Anais Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>tocador, premium, anais, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Tocador Silvi Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>tocador, silvi, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Tocador Multifuncional Birdie Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>tocador, multifuncional, birdie, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Tocador Multifuncional Birdie Grafito Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>tocador, multifuncional, birdie, grafito, muebles, gaudi, tocadores y percheros</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Tocador Multifuncional Birdie Muebles Gaudi</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>MUEBLES GAUDI</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Tocadores y Percheros</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>tocador, multifuncional, birdie, muebles, gaudi, tocadores y percheros</t>
         </is>
       </c>
     </row>

</xml_diff>